<commit_message>
Last data added, Burn-Down-Chart added
</commit_message>
<xml_diff>
--- a/doc/Backlog.xlsx
+++ b/doc/Backlog.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katerina Mlinaric\workspace\ch.bfh.btx8081.w2014.-team-green2-\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12288" windowHeight="6228" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23700" windowHeight="14000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Sprint 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Backlog Sprint 1 &amp; 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Backlog Sprint 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Burn-Down-Chart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
   <si>
     <t>ID</t>
   </si>
@@ -339,13 +340,34 @@
   </si>
   <si>
     <t>Katharina, Melisa,Manuel</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Updated</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,8 +392,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,10 +431,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -430,15 +469,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -476,19 +530,265 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Planned</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$B$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn-Down-Chart'!$B$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Updated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$B$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn-Down-Chart'!$B$8:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Burn-Down-Chart'!$B$6:$D$6</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Sprint 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Sprint 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sprint 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn-Down-Chart'!$B$9:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2133208168"/>
+        <c:axId val="2131118680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2133208168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2131118680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2131118680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2133208168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -538,11 +838,185 @@
         <a:p>
           <a:r>
             <a:rPr lang="de-DE" sz="1400"/>
-            <a:t>2.Sprint</a:t>
+            <a:t>2. Sprint</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Textfeld 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3449320"/>
+          <a:ext cx="13101320" cy="337820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400"/>
+            <a:t>1. Sprint</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3449320"/>
+          <a:ext cx="13101320" cy="337820"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400"/>
+            <a:t>3. Sprint</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -591,7 +1065,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -626,7 +1100,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -841,19 +1315,19 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="42.88671875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="5" customWidth="1"/>
     <col min="3" max="3" width="31.33203125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="5" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="28">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -879,7 +1353,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="28">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -905,7 +1379,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -931,7 +1405,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -957,7 +1431,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -983,7 +1457,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1009,7 +1483,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1035,41 +1509,46 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A3:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="7" customWidth="1"/>
     <col min="2" max="2" width="7" style="7" customWidth="1"/>
@@ -1077,410 +1556,357 @@
     <col min="4" max="4" width="24.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="23.6640625" style="7" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" style="7" customWidth="1"/>
-    <col min="11" max="11" width="16.88671875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13.5" style="7" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="3" spans="1:11" s="1" customFormat="1">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7">
+    <row r="4" spans="1:11" ht="36" customHeight="1">
+      <c r="A4" s="7">
         <v>1.1000000000000001</v>
-      </c>
-      <c r="B2" s="7">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="7">
-        <v>2</v>
-      </c>
-      <c r="J2" s="7">
-        <v>3</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7">
-        <v>1.2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="7">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7">
-        <v>4</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>1.3</v>
       </c>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="39.75" customHeight="1">
       <c r="A5" s="7">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5" s="7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="J5" s="7">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="28">
       <c r="A6" s="7">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="B6" s="7">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
       </c>
       <c r="I6" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="42">
       <c r="A7" s="7">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I7" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J7" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="28">
       <c r="A8" s="7">
-        <v>1.7</v>
+        <v>1.5</v>
       </c>
       <c r="B8" s="7">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="7">
+        <v>2</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>1</v>
+      </c>
+      <c r="J9" s="7">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7">
+        <v>1.7</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H10" s="7">
         <v>5</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I10" s="7">
         <v>3</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J10" s="7">
         <v>4</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="11">
+        <f>SUM(H4:H10)</f>
+        <v>15</v>
+      </c>
+      <c r="I11" s="11">
+        <f t="shared" ref="I11:J11" si="0">SUM(I4:I10)</f>
+        <v>13</v>
+      </c>
+      <c r="J11" s="11">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E13" s="8" t="s">
+      <c r="D15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F15" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G15" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H15" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K15" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+    <row r="19" spans="1:11">
+      <c r="A19" s="7">
         <v>2.1</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D19" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H19" s="7">
         <v>4</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I19" s="7">
         <v>6</v>
-      </c>
-      <c r="J17" s="7">
-        <v>5</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B18" s="7">
-        <v>2</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="7">
-        <v>2</v>
-      </c>
-      <c r="I18" s="7">
-        <v>6</v>
-      </c>
-      <c r="J18" s="7">
-        <v>8</v>
-      </c>
-      <c r="K18" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="B19" s="7">
-        <v>2</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="7">
-        <v>2</v>
-      </c>
-      <c r="I19" s="7">
-        <v>4</v>
       </c>
       <c r="J19" s="7">
         <v>5</v>
@@ -1489,24 +1915,24 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="28">
       <c r="A20" s="7">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B20" s="7">
         <v>2</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>5</v>
@@ -1515,222 +1941,339 @@
         <v>2</v>
       </c>
       <c r="I20" s="7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J20" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="28">
       <c r="A21" s="7">
-        <v>2.5</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B21" s="7">
         <v>2</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="G21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="7">
+        <v>2</v>
+      </c>
+      <c r="I21" s="7">
+        <v>4</v>
+      </c>
+      <c r="J21" s="7">
         <v>5</v>
-      </c>
-      <c r="H21" s="7">
-        <v>2</v>
-      </c>
-      <c r="I21" s="7">
-        <v>2</v>
-      </c>
-      <c r="J21" s="7">
-        <v>2</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="28">
       <c r="A22" s="7">
-        <v>2.6</v>
+        <v>2.4</v>
       </c>
       <c r="B22" s="7">
         <v>2</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H22" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I22" s="7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J22" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="28">
       <c r="A23" s="7">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="B23" s="7">
         <v>2</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="7">
+        <v>2</v>
+      </c>
+      <c r="I23" s="7">
+        <v>2</v>
+      </c>
+      <c r="J23" s="7">
+        <v>2</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="42">
+      <c r="A24" s="7">
+        <v>2.6</v>
+      </c>
+      <c r="B24" s="7">
+        <v>2</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="7">
+        <v>4</v>
+      </c>
+      <c r="I24" s="7">
         <v>6</v>
       </c>
-      <c r="H23" s="7">
-        <v>2</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>2.8</v>
-      </c>
-      <c r="B24" s="7">
-        <v>2</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="J24" s="7">
         <v>6</v>
-      </c>
-      <c r="H24" s="7">
-        <v>3</v>
-      </c>
-      <c r="I24" s="7">
-        <v>3</v>
-      </c>
-      <c r="J24" s="7">
-        <v>4</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K26" s="9"/>
-    </row>
-    <row r="29" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" ht="28">
+      <c r="A25" s="7">
+        <v>2.7</v>
+      </c>
+      <c r="B25" s="7">
+        <v>2</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="7">
+        <v>2</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="28">
+      <c r="A26" s="7">
+        <v>2.8</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="7">
+        <v>3</v>
+      </c>
+      <c r="I26" s="7">
+        <v>3</v>
+      </c>
+      <c r="J26" s="7">
+        <v>4</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11">
+      <c r="A27" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H27" s="11">
+        <f>SUM(H19:H26)</f>
+        <v>21</v>
+      </c>
+      <c r="I27" s="11">
+        <f t="shared" ref="I27:J27" si="1">SUM(I19:I26)</f>
+        <v>29</v>
+      </c>
+      <c r="J27" s="11">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="K28" s="9"/>
+    </row>
+    <row r="31" spans="1:11" ht="33" customHeight="1"/>
   </sheetData>
-  <conditionalFormatting sqref="K2:K7 K16 K18:K22 K24:K29 K9">
+  <conditionalFormatting sqref="K4:K9 K18 K20:K24 K26:K31 K11">
     <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="not started">
-      <formula>NOT(ISERROR(SEARCH("not started",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("not started",K4)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="finished">
-      <formula>NOT(ISERROR(SEARCH("finished",K2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("finished",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="11.5546875" style="3"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="5.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="21.6640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="1" spans="1:11" customFormat="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" customFormat="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="28">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="11" t="s">
+      <c r="D3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1743,7 +2286,7 @@
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1756,7 +2299,7 @@
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="42">
       <c r="A6" s="3">
         <v>3.1</v>
       </c>
@@ -1791,7 +2334,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="42">
       <c r="A7" s="3">
         <v>3.2</v>
       </c>
@@ -1826,7 +2369,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="42">
       <c r="A8" s="3">
         <v>3.3</v>
       </c>
@@ -1861,7 +2404,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="42">
       <c r="A9" s="3">
         <v>3.3</v>
       </c>
@@ -1896,7 +2439,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="42">
       <c r="A10" s="3">
         <v>3.4</v>
       </c>
@@ -1931,7 +2474,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="28">
       <c r="A11" s="3">
         <v>3.5</v>
       </c>
@@ -1966,7 +2509,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="28">
       <c r="A12" s="3">
         <v>3.6</v>
       </c>
@@ -2001,7 +2544,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="28">
       <c r="A13" s="3">
         <v>3.7</v>
       </c>
@@ -2036,8 +2579,218 @@
         <v>56</v>
       </c>
     </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="H14" s="12">
+        <f>SUM(H6:H13)</f>
+        <v>43</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" ref="I14:J14" si="0">SUM(I6:I13)</f>
+        <v>35</v>
+      </c>
+      <c r="J14" s="12">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2">
+        <f>'Backlog Sprint 1 &amp; 2'!H11</f>
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <f>'Backlog Sprint 1 &amp; 2'!H27</f>
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <f>'Backlog Sprint 3'!H14</f>
+        <v>43</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3">
+        <f>'Backlog Sprint 1 &amp; 2'!I11</f>
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <f>'Backlog Sprint 1 &amp; 2'!I27</f>
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <f>'Backlog Sprint 3'!I14</f>
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <f>SUM(B3:D3)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <f>'Backlog Sprint 1 &amp; 2'!J11</f>
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <f>'Backlog Sprint 1 &amp; 2'!J27</f>
+        <v>33</v>
+      </c>
+      <c r="D4">
+        <f>'Backlog Sprint 3'!J14</f>
+        <v>37</v>
+      </c>
+      <c r="E4">
+        <f>SUM(B4:D4)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B7">
+        <f>E2-B2</f>
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <f>B7-C2</f>
+        <v>43</v>
+      </c>
+      <c r="D7">
+        <f>C7-D2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8">
+        <f>E3-B3</f>
+        <v>64</v>
+      </c>
+      <c r="C8">
+        <f>B8-C3</f>
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <f>C8-D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9">
+        <f>E4-B4</f>
+        <v>70</v>
+      </c>
+      <c r="C9">
+        <f>B9-C4</f>
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <f>C9-D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" spans="2:2">
+      <c r="B23" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B16:B23"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>